<commit_message>
Updated Time Log 29-Sep
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26903"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nymta-my.sharepoint.com/personal/dorjan_mujollari_mtahq_org/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nymta-my.sharepoint.com/personal/dorjan_mujollari_mtahq_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2447BF10-8221-42BE-8D86-9152CE2565FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-240" windowWidth="29040" windowHeight="15840" xr2:uid="{46A880D0-B361-4B8F-90B7-862FAE06626B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -65,35 +65,82 @@
     <t>3.5h</t>
   </si>
   <si>
-    <t>Create page with information about the flu shot</t>
-  </si>
-  <si>
-    <t>Include the information provided and make sure the page is responsive to different devices while maintaning the design.</t>
-  </si>
-  <si>
-    <t>Site was ceated and made ready for User approval</t>
-  </si>
-  <si>
-    <t>New Department Conversion Pages</t>
-  </si>
-  <si>
-    <t>Migrate webpages from another depatment to the new intranet site.</t>
-  </si>
-  <si>
-    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site.</t>
-  </si>
-  <si>
     <t>8h</t>
   </si>
   <si>
     <t>5h</t>
+  </si>
+  <si>
+    <t>Based on feedback received, implemeted changes to create a new sample page</t>
+  </si>
+  <si>
+    <t>Created a new webpage containing information requested by the users.</t>
+  </si>
+  <si>
+    <t>Modifications made for better look and feel based on feedback. Aproved and pushed to production</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User priority task:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Create page with information about the flu shot</t>
+    </r>
+  </si>
+  <si>
+    <t>Include the information and make sure the page is responsive to different devices while maintaning the design.</t>
+  </si>
+  <si>
+    <t>New Divison Conversion Pages</t>
+  </si>
+  <si>
+    <t>Migrate webpages from another depatments division to the new intranet site.</t>
+  </si>
+  <si>
+    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site. Shreadsheet created for the legacy website containing all the pages and different links</t>
+  </si>
+  <si>
+    <t>Created a simple sample page</t>
+  </si>
+  <si>
+    <t>Another page created</t>
+  </si>
+  <si>
+    <t>More pages created</t>
+  </si>
+  <si>
+    <t>Received feedback on some of the pages, implemented changes and wating for more feedback</t>
+  </si>
+  <si>
+    <t>Presented the work done until now and received feedback</t>
+  </si>
+  <si>
+    <t>Implemented changes and created the last remaining pages.</t>
+  </si>
+  <si>
+    <t>Leaning Bootstrap and testing the knowledge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +156,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +173,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -167,15 +222,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -197,11 +308,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -517,107 +665,246 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D35DEF-D929-4362-ADF9-9ED6B03F5F4C}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" thickBot="1">
-      <c r="A2" s="3">
+    <row r="2" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>45180</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A3" s="3">
+    <row r="3" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>45181</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
         <v>45182</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10">
+        <v>45183</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>45184</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12">
+        <v>45187</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>45188</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10">
+        <v>45189</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90.75" customHeight="1" thickBot="1">
-      <c r="A4" s="3">
-        <v>45183</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A5" s="3">
-        <v>45184</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="D7" s="1"/>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>45190</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
+        <v>45191</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>45194</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12">
+        <v>45195</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12">
+        <v>45196</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
+        <v>45197</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45198</v>
+      </c>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+  <mergeCells count="6">
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B5:B15"/>
+    <mergeCell ref="C5:C15"/>
+    <mergeCell ref="D13:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Time Log Oct-9-2023
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nymta-my.sharepoint.com/personal/dorjan_mujollari_mtahq_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDB0822-A617-42B8-8786-29EA6AA21E0D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-240" windowWidth="29040" windowHeight="15840" xr2:uid="{46A880D0-B361-4B8F-90B7-862FAE06626B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,15 @@
   </si>
   <si>
     <t>Leaning Bootstrap and testing the knowledge</t>
+  </si>
+  <si>
+    <t>7h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created 2 different POC landing pages, connected to the main website, </t>
+  </si>
+  <si>
+    <t>Researched the page and best pratices for this division</t>
   </si>
 </sst>
 </file>
@@ -285,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,24 +341,27 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D35DEF-D929-4362-ADF9-9ED6B03F5F4C}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +688,7 @@
     <col min="1" max="1" width="31.85546875" style="14" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -753,7 +765,7 @@
       <c r="C5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="6" t="s">
@@ -764,9 +776,9 @@
       <c r="A6" s="10">
         <v>45184</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="18"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>10</v>
       </c>
@@ -775,8 +787,8 @@
       <c r="A7" s="12">
         <v>45187</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="8" t="s">
         <v>19</v>
       </c>
@@ -788,8 +800,8 @@
       <c r="A8" s="10">
         <v>45188</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
       <c r="D8" s="11" t="s">
         <v>11</v>
       </c>
@@ -801,8 +813,8 @@
       <c r="A9" s="10">
         <v>45189</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
       <c r="D9" s="8" t="s">
         <v>20</v>
       </c>
@@ -814,8 +826,8 @@
       <c r="A10" s="10">
         <v>45190</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
       <c r="D10" s="8" t="s">
         <v>21</v>
       </c>
@@ -827,8 +839,8 @@
       <c r="A11" s="10">
         <v>45191</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="13" t="s">
         <v>22</v>
       </c>
@@ -840,8 +852,8 @@
       <c r="A12" s="12">
         <v>45194</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
       <c r="D12" s="13" t="s">
         <v>23</v>
       </c>
@@ -853,8 +865,8 @@
       <c r="A13" s="12">
         <v>45195</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
       <c r="D13" s="19" t="s">
         <v>24</v>
       </c>
@@ -866,9 +878,9 @@
       <c r="A14" s="12">
         <v>45196</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="7" t="s">
         <v>8</v>
       </c>
@@ -888,8 +900,8 @@
       <c r="A16" s="2">
         <v>45198</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
       <c r="D16" s="5" t="s">
         <v>25</v>
       </c>
@@ -897,14 +909,105 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
+        <v>45201</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
+        <v>45202</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>45204</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>45205</v>
+      </c>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>45208</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="D17:D18"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="C5:C15"/>
     <mergeCell ref="D13:D15"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="C17:C21"/>
+    <mergeCell ref="D19:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Time Log Oct-20-2023
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nymta-my.sharepoint.com/personal/dorjan_mujollari_mtahq_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DDB0822-A617-42B8-8786-29EA6AA21E0D}"/>
+  <xr:revisionPtr revIDLastSave="183" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E943C45-ADA3-4B08-B75E-914B07488203}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-240" windowWidth="29040" windowHeight="15840" xr2:uid="{46A880D0-B361-4B8F-90B7-862FAE06626B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Include the information and make sure the page is responsive to different devices while maintaning the design.</t>
   </si>
   <si>
-    <t>New Divison Conversion Pages</t>
-  </si>
-  <si>
     <t>Migrate webpages from another depatments division to the new intranet site.</t>
   </si>
   <si>
@@ -143,6 +140,27 @@
   </si>
   <si>
     <t>Researched the page and best pratices for this division</t>
+  </si>
+  <si>
+    <t>Presented the work, made a few small changes, ready to be shown to the bussines owner</t>
+  </si>
+  <si>
+    <t>New information requested by the owner, made the requested changes.</t>
+  </si>
+  <si>
+    <t>Went over the whole department with supervisor, made the requested changes</t>
+  </si>
+  <si>
+    <t>Changes on the sub departments page layout made as requested, adding more content, added carusel images and content.</t>
+  </si>
+  <si>
+    <t>New Divison Conversion Pages (OpP)</t>
+  </si>
+  <si>
+    <t>New Divison Conversion Pages (BO)</t>
+  </si>
+  <si>
+    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site. Shreadsheet created for the legacy website containing all the pages and diffe</t>
   </si>
 </sst>
 </file>
@@ -182,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -290,11 +308,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -305,9 +332,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -317,12 +341,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -341,12 +359,12 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -354,13 +372,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,18 +698,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D35DEF-D929-4362-ADF9-9ED6B03F5F4C}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="33.140625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
@@ -701,7 +722,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -712,302 +733,382 @@
       <c r="A2" s="2">
         <v>45180</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45181</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10">
+      <c r="A4" s="7">
         <v>45182</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="11" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10">
+      <c r="A5" s="7">
         <v>45183</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="D5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>45184</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
+        <v>45187</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>45188</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10">
-        <v>45184</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="7" t="s">
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>45189</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>45190</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>45191</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12">
-        <v>45187</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="7" t="s">
+    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>45194</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10">
-        <v>45188</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="7" t="s">
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9">
+        <v>45195</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10">
-        <v>45189</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="6" t="s">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>45196</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10">
-        <v>45190</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="7" t="s">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12">
+        <v>45197</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10">
-        <v>45191</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12">
-        <v>45194</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12">
-        <v>45195</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="12">
-        <v>45196</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
-        <v>45197</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45198</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9">
+        <v>45201</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9">
+        <v>45202</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="7" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9">
+        <v>45204</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9">
+        <v>45205</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15">
-        <v>45201</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="6" t="s">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9">
+        <v>45208</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15">
-        <v>45202</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
-        <v>45204</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="15">
-        <v>45205</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15">
-        <v>45208</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>45209</v>
+      </c>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
+        <v>45211</v>
+      </c>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
+        <v>45212</v>
+      </c>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D24" s="21"/>
+      <c r="E24" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9">
+        <v>45215</v>
+      </c>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D25" s="21"/>
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>45216</v>
+      </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>45217</v>
+      </c>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
+      <c r="D27" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9">
+        <v>45218</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45219</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D17:D18"/>
+  <mergeCells count="12">
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B17:B28"/>
+    <mergeCell ref="C17:C28"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="C5:C15"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="B17:B21"/>
-    <mergeCell ref="C17:C21"/>
     <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Time Log Nov-01-2023
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nymta-my.sharepoint.com/personal/dorjan_mujollari_mtahq_org/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E943C45-ADA3-4B08-B75E-914B07488203}"/>
+  <xr:revisionPtr revIDLastSave="409" documentId="8_{E0FA940B-B322-4C5B-921C-AA9B8748EC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3782AA31-E889-424B-B028-255C7624D419}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-240" windowWidth="29040" windowHeight="15840" xr2:uid="{46A880D0-B361-4B8F-90B7-862FAE06626B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Work done</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Modify MyWifi site and Guideline for Telework site</t>
   </si>
   <si>
@@ -60,15 +57,6 @@
   </si>
   <si>
     <t>Sites were modifed to match the new design and logo was made transparent.</t>
-  </si>
-  <si>
-    <t>3.5h</t>
-  </si>
-  <si>
-    <t>8h</t>
-  </si>
-  <si>
-    <t>5h</t>
   </si>
   <si>
     <t>Based on feedback received, implemeted changes to create a new sample page</t>
@@ -127,15 +115,9 @@
     <t>Presented the work done until now and received feedback</t>
   </si>
   <si>
-    <t>Implemented changes and created the last remaining pages.</t>
-  </si>
-  <si>
     <t>Leaning Bootstrap and testing the knowledge</t>
   </si>
   <si>
-    <t>7h</t>
-  </si>
-  <si>
     <t xml:space="preserve">Created 2 different POC landing pages, connected to the main website, </t>
   </si>
   <si>
@@ -145,9 +127,6 @@
     <t>Presented the work, made a few small changes, ready to be shown to the bussines owner</t>
   </si>
   <si>
-    <t>New information requested by the owner, made the requested changes.</t>
-  </si>
-  <si>
     <t>Went over the whole department with supervisor, made the requested changes</t>
   </si>
   <si>
@@ -160,14 +139,47 @@
     <t>New Divison Conversion Pages (BO)</t>
   </si>
   <si>
-    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site. Shreadsheet created for the legacy website containing all the pages and diffe</t>
+    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site. Shreadsheet created for the legacy website containing all the pages and links. (waiting for design specifications to create POC)</t>
+  </si>
+  <si>
+    <t>New Divison Conversion Pages (DOS)</t>
+  </si>
+  <si>
+    <t>Familarized with the old website. Navigated through the content and made notes for broken links, old content or content that need to be reviewed or not included in the new site. Shreadsheet created for the legacy website containing all the pages and different links.</t>
+  </si>
+  <si>
+    <t>POC page and menu created</t>
+  </si>
+  <si>
+    <t>Time(hours)</t>
+  </si>
+  <si>
+    <t>New information requested by the owner, made the requested changes. Linked pages togethr through a top navigation menu.</t>
+  </si>
+  <si>
+    <t>Implemented changes and created the last remaining pages. Linked pages together through a top navigation menu.</t>
+  </si>
+  <si>
+    <t>More Pages created, combined them together though a top navigation menu</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Codding</t>
+  </si>
+  <si>
+    <t>Testing &amp; Debugging</t>
+  </si>
+  <si>
+    <t>Reasearch, Training,  Learning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,13 +203,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -321,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -338,9 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -366,6 +406,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -375,15 +436,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,21 +757,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D35DEF-D929-4362-ADF9-9ED6B03F5F4C}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" style="11" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" style="10" customWidth="1"/>
     <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="47" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,393 +783,541 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45180</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="H2" s="19"/>
+      <c r="I2" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45181</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="18">
+        <v>8</v>
+      </c>
+      <c r="H3" s="27"/>
+      <c r="I3" s="28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>45182</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="17">
+        <v>3.5</v>
+      </c>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>45183</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>45184</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>45187</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="E7" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
+        <v>45188</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>45189</v>
+      </c>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7">
-        <v>45182</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7">
-        <v>45183</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="E9" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>45190</v>
+      </c>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="E10" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>45191</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7">
-        <v>45184</v>
-      </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
-        <v>45187</v>
-      </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="8" t="s">
+      <c r="E11" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>45194</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>45188</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>45189</v>
-      </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>45190</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
-        <v>45191</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
-        <v>45194</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="E12" s="5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
         <v>45195</v>
       </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
         <v>45196</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="12">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11">
         <v>45197</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45198</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>45201</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>45202</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>45204</v>
+      </c>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>45205</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>45208</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>45209</v>
+      </c>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>45211</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>45212</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>45215</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>45216</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6">
+        <v>45217</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9">
-        <v>45201</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
-        <v>45202</v>
-      </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
-        <v>45204</v>
-      </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
-        <v>45205</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
-        <v>45208</v>
-      </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>45209</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
-        <v>45211</v>
-      </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
-        <v>45212</v>
-      </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9">
-        <v>45215</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>45216</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>45217</v>
-      </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="E27" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
         <v>45218</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="124.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45219</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11">
+        <v>45222</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45223</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="16">
+        <v>3.5</v>
+      </c>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="1:8" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45224</v>
+      </c>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="16">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11">
+        <v>45225</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E33" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11">
+        <v>45226</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E34" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="11">
+        <v>45229</v>
+      </c>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>10</v>
+      <c r="E35" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="11">
+        <v>45230</v>
+      </c>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11">
+        <v>45231</v>
+      </c>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="18">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11">
+        <v>45232</v>
+      </c>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11">
+        <v>45233</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="18">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="B17:B28"/>
-    <mergeCell ref="C17:C28"/>
+  <mergeCells count="19">
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B5:B15"/>
     <mergeCell ref="C5:C15"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D19:D21"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="B17:B28"/>
+    <mergeCell ref="C17:C28"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D35:D39"/>
+    <mergeCell ref="B31:B39"/>
+    <mergeCell ref="C31:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>